<commit_message>
fixed: 3hr subjs no longer overlapping schedules, but not getting set into any day with schedule in any timeframe position fixed: alertVariable error statements removed: coursetype from course offerings table
</commit_message>
<xml_diff>
--- a/static/files/subject_data2.xlsx
+++ b/static/files/subject_data2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jenze\Desktop\PROF LOADING CAPSTONE PROJECT\cbfsls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jenze\Desktop\PROF LOADING CAPSTONE PROJECT\NEWREPO\cbfsls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{446DDEB3-C161-4919-8394-332B18D581A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90090AAA-D644-41B9-BF3C-F831B3E9516E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{C503681A-46D2-4566-9B28-A025B06E37F5}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21990" windowHeight="13395" xr2:uid="{C503681A-46D2-4566-9B28-A025B06E37F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="69">
   <si>
     <t>NO.</t>
   </si>
@@ -40,6 +40,12 @@
   </si>
   <si>
     <t>UNITS</t>
+  </si>
+  <si>
+    <t>ROOMS</t>
+  </si>
+  <si>
+    <t>SECTIONS</t>
   </si>
   <si>
     <t>ECO 1</t>
@@ -319,7 +325,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -347,6 +353,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -667,21 +676,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22E8B8A1-8935-45EA-BFD9-F3E7AA710A9A}">
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" style="6" customWidth="1"/>
+    <col min="1" max="1" width="4.28515625" style="6" customWidth="1"/>
     <col min="2" max="2" width="15.28515625" style="6" customWidth="1"/>
     <col min="3" max="3" width="49.7109375" style="6" customWidth="1"/>
     <col min="4" max="4" width="30.28515625" style="6" customWidth="1"/>
     <col min="5" max="5" width="13.140625" style="6" customWidth="1"/>
-    <col min="6" max="6" width="27.28515625" style="6" customWidth="1"/>
-    <col min="7" max="7" width="22" style="6" customWidth="1"/>
-    <col min="8" max="8" width="21" style="6" customWidth="1"/>
-    <col min="9" max="16384" width="8.85546875" style="6"/>
+    <col min="6" max="6" width="15.5703125" style="6" customWidth="1"/>
+    <col min="7" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15">
@@ -701,10 +708,14 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
+        <v>66</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" spans="1:8" ht="15">
       <c r="A2" s="5"/>
@@ -712,7 +723,7 @@
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
-      <c r="F2" s="5"/>
+      <c r="F2" s="1"/>
       <c r="G2" s="3"/>
       <c r="H2" s="1"/>
     </row>
@@ -722,379 +733,378 @@
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
-      <c r="F3" s="5"/>
+      <c r="F3" s="1"/>
       <c r="G3" s="3"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" ht="15">
       <c r="A4" s="5">
         <v>1</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E4" s="5">
         <v>3</v>
       </c>
-      <c r="F4" s="5" t="s">
-        <v>65</v>
+      <c r="F4" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="G4" s="8"/>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" ht="15">
       <c r="A5" s="5">
         <v>2</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C5" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>7</v>
-      </c>
       <c r="E5" s="5">
         <v>3</v>
       </c>
-      <c r="F5" s="5" t="s">
-        <v>65</v>
+      <c r="F5" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="G5" s="8"/>
       <c r="H5" s="5"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" ht="15">
       <c r="A6" s="5">
         <v>3</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E6" s="5">
         <v>3</v>
       </c>
-      <c r="F6" s="5" t="s">
-        <v>65</v>
+      <c r="F6" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="G6" s="8"/>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" ht="15">
       <c r="A7" s="5">
         <v>4</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E7" s="5">
         <v>3</v>
       </c>
-      <c r="F7" s="5" t="s">
-        <v>65</v>
+      <c r="F7" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="G7" s="8"/>
       <c r="H7" s="5"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" ht="15">
       <c r="A8" s="5">
         <v>5</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E8" s="5">
         <v>3</v>
       </c>
-      <c r="F8" s="5" t="s">
-        <v>65</v>
+      <c r="F8" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="G8" s="8"/>
       <c r="H8" s="5"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" ht="15">
       <c r="A9" s="5">
         <v>6</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E9" s="5">
         <v>3</v>
       </c>
-      <c r="F9" s="5" t="s">
-        <v>65</v>
+      <c r="F9" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="G9" s="8"/>
       <c r="H9" s="5"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" ht="15">
       <c r="A10" s="5">
         <v>7</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E10" s="5">
         <v>3</v>
       </c>
-      <c r="F10" s="5" t="s">
-        <v>65</v>
+      <c r="F10" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="G10" s="8"/>
       <c r="H10" s="5"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" ht="15">
       <c r="A11" s="5">
         <v>8</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E11" s="5">
         <v>3</v>
       </c>
-      <c r="F11" s="5" t="s">
-        <v>65</v>
+      <c r="F11" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="G11" s="8"/>
       <c r="H11" s="5"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" ht="15">
       <c r="A12" s="5">
         <v>9</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E12" s="5">
         <v>2</v>
       </c>
-      <c r="F12" s="5" t="s">
-        <v>65</v>
+      <c r="F12" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="G12" s="8"/>
       <c r="H12" s="5"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" ht="15">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="9"/>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
-      <c r="F13" s="5" t="s">
-        <v>65</v>
-      </c>
+      <c r="F13" s="1"/>
       <c r="G13" s="8"/>
       <c r="H13" s="5"/>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" ht="15">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="9"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
+      <c r="F14" s="10"/>
       <c r="G14" s="8"/>
       <c r="H14" s="5"/>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" ht="15">
       <c r="A15" s="5">
         <v>10</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E15" s="8">
         <v>3</v>
       </c>
-      <c r="F15" s="5" t="s">
-        <v>65</v>
+      <c r="F15" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="G15" s="8"/>
       <c r="H15" s="5"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" ht="15">
       <c r="A16" s="5">
         <v>11</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C16" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>28</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>26</v>
       </c>
       <c r="E16" s="5">
         <v>6</v>
       </c>
-      <c r="F16" s="5" t="s">
-        <v>65</v>
+      <c r="F16" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="G16" s="8"/>
       <c r="H16" s="5"/>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" ht="15">
       <c r="A17" s="5">
         <v>12</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E17" s="5">
         <v>3</v>
       </c>
-      <c r="F17" s="5" t="s">
-        <v>65</v>
+      <c r="F17" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="G17" s="8"/>
       <c r="H17" s="5"/>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" ht="15">
       <c r="A18" s="5">
         <v>13</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E18" s="5">
         <v>3</v>
       </c>
-      <c r="F18" s="5" t="s">
-        <v>65</v>
+      <c r="F18" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="G18" s="8"/>
       <c r="H18" s="5"/>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" ht="15">
       <c r="A19" s="5">
         <v>14</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E19" s="5">
         <v>3</v>
       </c>
-      <c r="F19" s="5" t="s">
-        <v>65</v>
+      <c r="F19" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="G19" s="8"/>
       <c r="H19" s="5"/>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" ht="15">
       <c r="A20" s="5">
         <v>15</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E20" s="5">
         <v>3</v>
       </c>
-      <c r="F20" s="5" t="s">
-        <v>65</v>
+      <c r="F20" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="G20" s="8"/>
       <c r="H20" s="5"/>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" ht="15">
       <c r="A21" s="5">
         <v>16</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E21" s="5">
         <v>3</v>
       </c>
-      <c r="F21" s="5" t="s">
-        <v>65</v>
+      <c r="F21" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="G21" s="8"/>
       <c r="H21" s="5"/>
@@ -1104,19 +1114,19 @@
         <v>17</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>40</v>
+        <v>41</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>42</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E22" s="5">
         <v>3</v>
       </c>
-      <c r="F22" s="5" t="s">
-        <v>65</v>
+      <c r="F22" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="G22" s="8"/>
       <c r="H22" s="5"/>
@@ -1126,219 +1136,217 @@
         <v>18</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E23" s="5">
         <v>2</v>
       </c>
-      <c r="F23" s="5" t="s">
-        <v>65</v>
+      <c r="F23" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="G23" s="8"/>
       <c r="H23" s="5"/>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" ht="15">
       <c r="A24" s="5"/>
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
-      <c r="F24" s="5" t="s">
-        <v>65</v>
-      </c>
+      <c r="F24" s="1"/>
       <c r="G24" s="8"/>
       <c r="H24" s="5"/>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" ht="15">
       <c r="A25" s="5">
         <v>19</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E25" s="8">
         <v>3</v>
       </c>
-      <c r="F25" s="5" t="s">
-        <v>65</v>
+      <c r="F25" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="G25" s="8"/>
       <c r="H25" s="5"/>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" ht="15">
       <c r="A26" s="5">
         <v>20</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E26" s="8">
         <v>3</v>
       </c>
-      <c r="F26" s="5" t="s">
-        <v>65</v>
+      <c r="F26" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="G26" s="8"/>
       <c r="H26" s="5"/>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" ht="15">
       <c r="A27" s="5">
         <v>21</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E27" s="8">
         <v>3</v>
       </c>
-      <c r="F27" s="5" t="s">
-        <v>65</v>
+      <c r="F27" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="G27" s="8"/>
       <c r="H27" s="8"/>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" ht="15">
       <c r="A28" s="5">
         <v>22</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E28" s="8">
         <v>3</v>
       </c>
-      <c r="F28" s="5" t="s">
-        <v>65</v>
+      <c r="F28" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="G28" s="8"/>
       <c r="H28" s="5"/>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" ht="15">
       <c r="A29" s="5">
         <v>23</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E29" s="8">
         <v>3</v>
       </c>
-      <c r="F29" s="5" t="s">
-        <v>65</v>
+      <c r="F29" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="G29" s="8"/>
       <c r="H29" s="5"/>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" ht="15">
       <c r="A30" s="5">
         <v>24</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E30" s="8">
         <v>3</v>
       </c>
-      <c r="F30" s="5" t="s">
-        <v>65</v>
+      <c r="F30" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="G30" s="8"/>
       <c r="H30" s="5"/>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" ht="15">
       <c r="A31" s="5">
         <v>25</v>
       </c>
       <c r="B31" s="8" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C31" s="8" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E31" s="8">
         <v>3</v>
       </c>
-      <c r="F31" s="5" t="s">
-        <v>65</v>
+      <c r="F31" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="G31" s="8"/>
       <c r="H31" s="5"/>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" ht="15">
       <c r="A32" s="5">
         <v>26</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C32" s="8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="E32" s="8">
         <v>3</v>
       </c>
-      <c r="F32" s="5" t="s">
-        <v>65</v>
+      <c r="F32" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="G32" s="8"/>
       <c r="H32" s="5"/>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" ht="15">
       <c r="A33" s="5"/>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
       <c r="E33" s="5"/>
-      <c r="F33" s="5" t="s">
-        <v>65</v>
+      <c r="F33" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="G33" s="8"/>
       <c r="H33" s="5"/>
@@ -1348,56 +1356,56 @@
         <v>26</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C34" s="8" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E34" s="5">
         <v>3</v>
       </c>
-      <c r="F34" s="5" t="s">
-        <v>65</v>
+      <c r="F34" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="G34" s="8"/>
       <c r="H34" s="5"/>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" ht="15">
       <c r="A35" s="5">
         <v>27</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C35" s="8" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E35" s="5">
         <v>6</v>
       </c>
-      <c r="F35" s="5" t="s">
-        <v>65</v>
+      <c r="F35" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="G35" s="8"/>
       <c r="H35" s="5"/>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" ht="15">
       <c r="A36" s="5"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
       <c r="D36" s="5"/>
       <c r="E36" s="4"/>
-      <c r="F36" s="5"/>
+      <c r="F36" s="1"/>
       <c r="G36" s="5"/>
       <c r="H36" s="5"/>
     </row>
-    <row r="37" spans="1:8" ht="15" customHeight="1">
+    <row r="37" spans="1:8" ht="15">
       <c r="A37" s="5"/>
       <c r="B37" s="5"/>
       <c r="C37" s="9"/>

</xml_diff>